<commit_message>
Starting Introduction in english
</commit_message>
<xml_diff>
--- a/Certification CDA/Recap_Compétences.xlsx
+++ b/Certification CDA/Recap_Compétences.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\EPSI\Certif_CDA_Contenue\Certification CDA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D810E83-2FD7-412F-9D3E-7B8948847EAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB2435E5-7B7C-4745-8AA8-0D350C9EE6F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" xr2:uid="{AAD9A9D6-F1C0-4B06-9435-EEE062357DBD}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="64">
   <si>
     <t>Compétences professionnelles</t>
   </si>
@@ -217,6 +217,9 @@
   </si>
   <si>
     <t>Prisearch</t>
+  </si>
+  <si>
+    <t>Airsens</t>
   </si>
 </sst>
 </file>
@@ -509,42 +512,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="9" xfId="2" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -555,6 +522,42 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="10" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -563,7 +566,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Note" xfId="3" builtinId="10"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="2">
     <dxf>
       <fill>
         <patternFill>
@@ -575,20 +578,6 @@
       <fill>
         <patternFill>
           <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
     </dxf>
@@ -947,24 +936,24 @@
       <c r="H1" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="J1" s="27" t="s">
+      <c r="J1" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="L1" s="31" t="s">
+      <c r="L1" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="M1" s="30" t="s">
+      <c r="M1" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="N1" s="30" t="s">
+      <c r="N1" s="18" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="15">
+      <c r="A2" s="20">
         <v>1</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="23" t="s">
         <v>8</v>
       </c>
       <c r="C2" s="5">
@@ -985,18 +974,18 @@
       <c r="H2" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="28"/>
-      <c r="L2" s="29"/>
-      <c r="M2" s="30" t="s">
+      <c r="J2" s="16"/>
+      <c r="L2" s="17"/>
+      <c r="M2" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="N2" s="30" t="s">
+      <c r="N2" s="18" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:14" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="16"/>
-      <c r="B3" s="19"/>
+      <c r="A3" s="21"/>
+      <c r="B3" s="24"/>
       <c r="C3" s="5">
         <v>2</v>
       </c>
@@ -1015,18 +1004,18 @@
       <c r="H3" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="J3" s="28"/>
-      <c r="L3" s="29"/>
-      <c r="M3" s="30" t="s">
+      <c r="J3" s="16"/>
+      <c r="L3" s="17"/>
+      <c r="M3" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="N3" s="30" t="s">
+      <c r="N3" s="18" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:14" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="16"/>
-      <c r="B4" s="19"/>
+      <c r="A4" s="21"/>
+      <c r="B4" s="24"/>
       <c r="C4" s="5">
         <v>3</v>
       </c>
@@ -1043,18 +1032,18 @@
       <c r="H4" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="J4" s="28"/>
-      <c r="L4" s="29"/>
-      <c r="M4" s="30" t="s">
+      <c r="J4" s="16"/>
+      <c r="L4" s="17"/>
+      <c r="M4" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="N4" s="30" t="s">
+      <c r="N4" s="18" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="16"/>
-      <c r="B5" s="19"/>
+      <c r="A5" s="21"/>
+      <c r="B5" s="24"/>
       <c r="C5" s="5">
         <v>4</v>
       </c>
@@ -1073,14 +1062,16 @@
       <c r="H5" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="J5" s="28"/>
-      <c r="L5" s="29"/>
-      <c r="M5" s="29"/>
-      <c r="N5" s="29"/>
+      <c r="J5" s="16"/>
+      <c r="L5" s="17"/>
+      <c r="M5" s="17"/>
+      <c r="N5" s="18" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="6" spans="1:14" ht="37.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="17"/>
-      <c r="B6" s="20"/>
+      <c r="A6" s="22"/>
+      <c r="B6" s="25"/>
       <c r="C6" s="5">
         <v>5</v>
       </c>
@@ -1099,16 +1090,16 @@
       <c r="H6" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="J6" s="28"/>
-      <c r="L6" s="29"/>
-      <c r="M6" s="29"/>
-      <c r="N6" s="29"/>
+      <c r="J6" s="16"/>
+      <c r="L6" s="17"/>
+      <c r="M6" s="17"/>
+      <c r="N6" s="17"/>
     </row>
     <row r="7" spans="1:14" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="21">
+      <c r="A7" s="26">
         <v>2</v>
       </c>
-      <c r="B7" s="24" t="s">
+      <c r="B7" s="29" t="s">
         <v>14</v>
       </c>
       <c r="C7" s="10">
@@ -1129,14 +1120,14 @@
       <c r="H7" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="J7" s="28"/>
-      <c r="L7" s="29"/>
-      <c r="M7" s="29"/>
-      <c r="N7" s="29"/>
+      <c r="J7" s="16"/>
+      <c r="L7" s="17"/>
+      <c r="M7" s="17"/>
+      <c r="N7" s="17"/>
     </row>
     <row r="8" spans="1:14" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="22"/>
-      <c r="B8" s="25"/>
+      <c r="A8" s="27"/>
+      <c r="B8" s="30"/>
       <c r="C8" s="10">
         <v>7</v>
       </c>
@@ -1155,14 +1146,14 @@
       <c r="H8" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="J8" s="28"/>
-      <c r="L8" s="29"/>
-      <c r="M8" s="29"/>
-      <c r="N8" s="29"/>
+      <c r="J8" s="16"/>
+      <c r="L8" s="17"/>
+      <c r="M8" s="17"/>
+      <c r="N8" s="17"/>
     </row>
     <row r="9" spans="1:14" ht="37.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="23"/>
-      <c r="B9" s="26"/>
+      <c r="A9" s="28"/>
+      <c r="B9" s="31"/>
       <c r="C9" s="10">
         <v>8</v>
       </c>
@@ -1181,16 +1172,16 @@
       <c r="H9" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="J9" s="28"/>
-      <c r="L9" s="29"/>
-      <c r="M9" s="29"/>
-      <c r="N9" s="29"/>
+      <c r="J9" s="16"/>
+      <c r="L9" s="17"/>
+      <c r="M9" s="17"/>
+      <c r="N9" s="17"/>
     </row>
     <row r="10" spans="1:14" ht="64.900000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="21">
+      <c r="A10" s="26">
         <v>3</v>
       </c>
-      <c r="B10" s="18" t="s">
+      <c r="B10" s="23" t="s">
         <v>18</v>
       </c>
       <c r="C10" s="5">
@@ -1211,14 +1202,14 @@
       <c r="H10" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="J10" s="28"/>
-      <c r="L10" s="29"/>
-      <c r="M10" s="29"/>
-      <c r="N10" s="29"/>
+      <c r="J10" s="16"/>
+      <c r="L10" s="17"/>
+      <c r="M10" s="17"/>
+      <c r="N10" s="17"/>
     </row>
     <row r="11" spans="1:14" ht="37.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="22"/>
-      <c r="B11" s="19"/>
+      <c r="A11" s="27"/>
+      <c r="B11" s="24"/>
       <c r="C11" s="5">
         <v>10</v>
       </c>
@@ -1237,14 +1228,14 @@
       <c r="H11" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="J11" s="28"/>
-      <c r="L11" s="29"/>
-      <c r="M11" s="29"/>
-      <c r="N11" s="29"/>
+      <c r="J11" s="16"/>
+      <c r="L11" s="17"/>
+      <c r="M11" s="17"/>
+      <c r="N11" s="17"/>
     </row>
     <row r="12" spans="1:14" ht="37.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="22"/>
-      <c r="B12" s="19"/>
+      <c r="A12" s="27"/>
+      <c r="B12" s="24"/>
       <c r="C12" s="5">
         <v>11</v>
       </c>
@@ -1263,14 +1254,14 @@
       <c r="H12" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="J12" s="28"/>
-      <c r="L12" s="29"/>
-      <c r="M12" s="29"/>
-      <c r="N12" s="29"/>
+      <c r="J12" s="16"/>
+      <c r="L12" s="17"/>
+      <c r="M12" s="17"/>
+      <c r="N12" s="17"/>
     </row>
     <row r="13" spans="1:14" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="22"/>
-      <c r="B13" s="19"/>
+      <c r="A13" s="27"/>
+      <c r="B13" s="24"/>
       <c r="C13" s="5">
         <v>12</v>
       </c>
@@ -1289,14 +1280,14 @@
       <c r="H13" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="J13" s="28"/>
-      <c r="L13" s="29"/>
-      <c r="M13" s="29"/>
-      <c r="N13" s="29"/>
+      <c r="J13" s="16"/>
+      <c r="L13" s="17"/>
+      <c r="M13" s="17"/>
+      <c r="N13" s="17"/>
     </row>
     <row r="14" spans="1:14" ht="37.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="22"/>
-      <c r="B14" s="19"/>
+      <c r="A14" s="27"/>
+      <c r="B14" s="24"/>
       <c r="C14" s="5">
         <v>13</v>
       </c>
@@ -1315,14 +1306,14 @@
       <c r="H14" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="J14" s="28"/>
-      <c r="L14" s="29"/>
-      <c r="M14" s="29"/>
-      <c r="N14" s="29"/>
+      <c r="J14" s="16"/>
+      <c r="L14" s="17"/>
+      <c r="M14" s="17"/>
+      <c r="N14" s="17"/>
     </row>
     <row r="15" spans="1:14" ht="37.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="22"/>
-      <c r="B15" s="19"/>
+      <c r="A15" s="27"/>
+      <c r="B15" s="24"/>
       <c r="C15" s="5">
         <v>14</v>
       </c>
@@ -1341,14 +1332,14 @@
       <c r="H15" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="J15" s="28"/>
-      <c r="L15" s="29"/>
-      <c r="M15" s="29"/>
-      <c r="N15" s="29"/>
+      <c r="J15" s="16"/>
+      <c r="L15" s="17"/>
+      <c r="M15" s="17"/>
+      <c r="N15" s="17"/>
     </row>
     <row r="16" spans="1:14" ht="217.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="23"/>
-      <c r="B16" s="20"/>
+      <c r="A16" s="28"/>
+      <c r="B16" s="25"/>
       <c r="C16" s="5">
         <v>15</v>
       </c>
@@ -1367,10 +1358,10 @@
       <c r="H16" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="J16" s="28"/>
-      <c r="L16" s="29"/>
-      <c r="M16" s="29"/>
-      <c r="N16" s="29"/>
+      <c r="J16" s="16"/>
+      <c r="L16" s="17"/>
+      <c r="M16" s="17"/>
+      <c r="N16" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -1381,20 +1372,12 @@
     <mergeCell ref="B7:B9"/>
     <mergeCell ref="B10:B16"/>
   </mergeCells>
-  <conditionalFormatting sqref="C2:H2">
-    <cfRule type="expression" dxfId="3" priority="6">
-      <formula>$H2="Oui"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="2" priority="3">
+  <conditionalFormatting sqref="C2:H16">
+    <cfRule type="expression" dxfId="1" priority="1">
       <formula>$H2="A finir"</formula>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C3:H16">
-    <cfRule type="expression" dxfId="1" priority="1">
-      <formula>$H3="A finir"</formula>
-    </cfRule>
     <cfRule type="expression" dxfId="0" priority="2">
-      <formula>$H3="Oui"</formula>
+      <formula>$H2="Oui"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Structure almost fini | TDM Finish
</commit_message>
<xml_diff>
--- a/Certification CDA/Recap_Compétences.xlsx
+++ b/Certification CDA/Recap_Compétences.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\EPSI\Certif_CDA_Contenue\Certification CDA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lilia\Desktop\EPSI\Certif_CDA_Contenue\Certification CDA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB2435E5-7B7C-4745-8AA8-0D350C9EE6F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D20D63E-691D-4B18-B0D1-CF8C35499B77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" xr2:uid="{AAD9A9D6-F1C0-4B06-9435-EEE062357DBD}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{AAD9A9D6-F1C0-4B06-9435-EEE062357DBD}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="66">
   <si>
     <t>Compétences professionnelles</t>
   </si>
@@ -220,6 +220,13 @@
   </si>
   <si>
     <t>Airsens</t>
+  </si>
+  <si>
+    <t>Rédiger une documentation
+ pour chaque applications</t>
+  </si>
+  <si>
+    <t>VITAM</t>
   </si>
 </sst>
 </file>
@@ -893,25 +900,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3489122-4D15-4F26-9748-79BCEDC1CFA9}">
   <dimension ref="A1:N16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.85546875" customWidth="1"/>
+    <col min="1" max="1" width="4.88671875" customWidth="1"/>
     <col min="2" max="2" width="28" customWidth="1"/>
-    <col min="4" max="4" width="50.7109375" customWidth="1"/>
-    <col min="5" max="5" width="18.85546875" customWidth="1"/>
-    <col min="6" max="6" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="53.28515625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="17.42578125" customWidth="1"/>
-    <col min="12" max="12" width="17.85546875" customWidth="1"/>
-    <col min="13" max="13" width="18.42578125" customWidth="1"/>
-    <col min="14" max="14" width="20.140625" customWidth="1"/>
+    <col min="4" max="4" width="50.6640625" customWidth="1"/>
+    <col min="5" max="5" width="18.88671875" customWidth="1"/>
+    <col min="6" max="6" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="53.33203125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="17.44140625" customWidth="1"/>
+    <col min="9" max="9" width="31.109375" customWidth="1"/>
+    <col min="12" max="12" width="17.88671875" customWidth="1"/>
+    <col min="13" max="13" width="18.44140625" customWidth="1"/>
+    <col min="14" max="14" width="20.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="2" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" s="2" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -949,7 +957,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="20">
         <v>1</v>
       </c>
@@ -983,7 +991,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="21"/>
       <c r="B3" s="24"/>
       <c r="C3" s="5">
@@ -1004,6 +1012,9 @@
       <c r="H3" s="8" t="s">
         <v>31</v>
       </c>
+      <c r="I3" s="1" t="s">
+        <v>64</v>
+      </c>
       <c r="J3" s="16"/>
       <c r="L3" s="17"/>
       <c r="M3" s="18" t="s">
@@ -1013,7 +1024,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="21"/>
       <c r="B4" s="24"/>
       <c r="C4" s="5">
@@ -1041,7 +1052,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="21"/>
       <c r="B5" s="24"/>
       <c r="C5" s="5">
@@ -1064,12 +1075,14 @@
       </c>
       <c r="J5" s="16"/>
       <c r="L5" s="17"/>
-      <c r="M5" s="17"/>
+      <c r="M5" s="18" t="s">
+        <v>65</v>
+      </c>
       <c r="N5" s="18" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="37.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" ht="37.200000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="22"/>
       <c r="B6" s="25"/>
       <c r="C6" s="5">
@@ -1095,7 +1108,7 @@
       <c r="M6" s="17"/>
       <c r="N6" s="17"/>
     </row>
-    <row r="7" spans="1:14" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="26">
         <v>2</v>
       </c>
@@ -1125,7 +1138,7 @@
       <c r="M7" s="17"/>
       <c r="N7" s="17"/>
     </row>
-    <row r="8" spans="1:14" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="27"/>
       <c r="B8" s="30"/>
       <c r="C8" s="10">
@@ -1151,7 +1164,7 @@
       <c r="M8" s="17"/>
       <c r="N8" s="17"/>
     </row>
-    <row r="9" spans="1:14" ht="37.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" ht="37.200000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="28"/>
       <c r="B9" s="31"/>
       <c r="C9" s="10">
@@ -1177,7 +1190,7 @@
       <c r="M9" s="17"/>
       <c r="N9" s="17"/>
     </row>
-    <row r="10" spans="1:14" ht="64.900000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" ht="64.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="26">
         <v>3</v>
       </c>
@@ -1207,7 +1220,7 @@
       <c r="M10" s="17"/>
       <c r="N10" s="17"/>
     </row>
-    <row r="11" spans="1:14" ht="37.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" ht="37.200000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="27"/>
       <c r="B11" s="24"/>
       <c r="C11" s="5">
@@ -1233,7 +1246,7 @@
       <c r="M11" s="17"/>
       <c r="N11" s="17"/>
     </row>
-    <row r="12" spans="1:14" ht="37.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" ht="37.200000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="27"/>
       <c r="B12" s="24"/>
       <c r="C12" s="5">
@@ -1259,7 +1272,7 @@
       <c r="M12" s="17"/>
       <c r="N12" s="17"/>
     </row>
-    <row r="13" spans="1:14" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="27"/>
       <c r="B13" s="24"/>
       <c r="C13" s="5">
@@ -1285,7 +1298,7 @@
       <c r="M13" s="17"/>
       <c r="N13" s="17"/>
     </row>
-    <row r="14" spans="1:14" ht="37.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" ht="37.200000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="27"/>
       <c r="B14" s="24"/>
       <c r="C14" s="5">
@@ -1311,7 +1324,7 @@
       <c r="M14" s="17"/>
       <c r="N14" s="17"/>
     </row>
-    <row r="15" spans="1:14" ht="37.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" ht="37.200000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="27"/>
       <c r="B15" s="24"/>
       <c r="C15" s="5">
@@ -1337,7 +1350,7 @@
       <c r="M15" s="17"/>
       <c r="N15" s="17"/>
     </row>
-    <row r="16" spans="1:14" ht="217.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" ht="217.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="28"/>
       <c r="B16" s="25"/>
       <c r="C16" s="5">

</xml_diff>